<commit_message>
Se generaron los dos mapas con votos de candidatos discrecionales. Falta estandarizar las escalas de las paletas de colores.
</commit_message>
<xml_diff>
--- a/idh_censo17.xlsx
+++ b/idh_censo17.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jair Alva\Desktop\REDES\Columnas de opinión\Candidatos discrecionales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529B5326-B0E1-490A-B6D3-B732E11AAE3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8338C73B-35D6-4A0E-9278-5081DEDC6831}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mjd1HfygFeTET/U9WkGrGZLvTSuLA=="/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="394">
   <si>
     <t>Provincia</t>
   </si>
@@ -231,9 +231,6 @@
     <t>070100</t>
   </si>
   <si>
-    <t>Provincia Constitucional del Callao</t>
-  </si>
-  <si>
     <t>080100</t>
   </si>
   <si>
@@ -621,591 +618,6 @@
     <t>250400</t>
   </si>
   <si>
-    <t>Amazonas, provincia: Chachapoyas</t>
-  </si>
-  <si>
-    <t>Amazonas, provincia: Bagua</t>
-  </si>
-  <si>
-    <t>Amazonas, provincia: Bongara</t>
-  </si>
-  <si>
-    <t>Amazonas, provincia: Condorcanqui</t>
-  </si>
-  <si>
-    <t>Amazonas, provincia: Luya</t>
-  </si>
-  <si>
-    <t>Amazonas, provincia: Rodríguez de Mendoza</t>
-  </si>
-  <si>
-    <t>Amazonas, provincia: Utcubamba</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Huaraz</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Aija</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Antonio Raymondi</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Asunción</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Bolognesi</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Carhuaz</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Carlos Fermín Fitzcarrald</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Casma</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Corongo</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Huari</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Huarmey</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Huaylas</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Mariscal Luzuriaga</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Ocros</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Pallasca</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Pomabamba</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Recuay</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Santa</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Sihuas</t>
-  </si>
-  <si>
-    <t>Áncash, provincia: Yungay</t>
-  </si>
-  <si>
-    <t>Apurímac, provincia: Abancay</t>
-  </si>
-  <si>
-    <t>Apurímac, provincia: Andahuaylas</t>
-  </si>
-  <si>
-    <t>Apurímac, provincia: Antabamba</t>
-  </si>
-  <si>
-    <t>Apurímac, provincia: Aymaraes</t>
-  </si>
-  <si>
-    <t>Apurímac, provincia: Cotabambas</t>
-  </si>
-  <si>
-    <t>Apurímac, provincia: Chincheros</t>
-  </si>
-  <si>
-    <t>Apurímac, provincia: Grau</t>
-  </si>
-  <si>
-    <t>Arequipa, provincia: Arequipa</t>
-  </si>
-  <si>
-    <t>Arequipa, provincia: Camaná</t>
-  </si>
-  <si>
-    <t>Arequipa, provincia: Caravelí</t>
-  </si>
-  <si>
-    <t>Arequipa, provincia: Castilla</t>
-  </si>
-  <si>
-    <t>Arequipa, provincia: Caylloma</t>
-  </si>
-  <si>
-    <t>Arequipa, provincia: Condesuyos</t>
-  </si>
-  <si>
-    <t>Arequipa, provincia: Islay</t>
-  </si>
-  <si>
-    <t>Arequipa, provincia: La Unión</t>
-  </si>
-  <si>
-    <t>Ayacucho, provincia: Huamanga</t>
-  </si>
-  <si>
-    <t>Ayacucho, provincia: Cangallo</t>
-  </si>
-  <si>
-    <t>Ayacucho, provincia: Huanca Sancos</t>
-  </si>
-  <si>
-    <t>Ayacucho, provincia: Huanta</t>
-  </si>
-  <si>
-    <t>Ayacucho, provincia: La Mar</t>
-  </si>
-  <si>
-    <t>Ayacucho, provincia: Lucanas</t>
-  </si>
-  <si>
-    <t>Ayacucho, provincia: Parinacochas</t>
-  </si>
-  <si>
-    <t>Ayacucho, provincia: Páucar del Sara Sara</t>
-  </si>
-  <si>
-    <t>Ayacucho, provincia: Sucre</t>
-  </si>
-  <si>
-    <t>Ayacucho, provincia: Víctor Fajardo</t>
-  </si>
-  <si>
-    <t>Ayacucho, provincia: Vilcas Huamán</t>
-  </si>
-  <si>
-    <t>Cajamarca, provincia: Cajamarca</t>
-  </si>
-  <si>
-    <t>Cajamarca, provincia: Cajabamba</t>
-  </si>
-  <si>
-    <t>Cajamarca, provincia: Celendín</t>
-  </si>
-  <si>
-    <t>Cajamarca, provincia: Chota</t>
-  </si>
-  <si>
-    <t>Cajamarca, provincia: Contumazá</t>
-  </si>
-  <si>
-    <t>Cajamarca, provincia: Cutervo</t>
-  </si>
-  <si>
-    <t>Cajamarca, provincia: Hualgayoc</t>
-  </si>
-  <si>
-    <t>Cajamarca, provincia: Jaén</t>
-  </si>
-  <si>
-    <t>Cajamarca, provincia: San Ignacio</t>
-  </si>
-  <si>
-    <t>Cajamarca, provincia: San Marcos</t>
-  </si>
-  <si>
-    <t>Cajamarca, provincia: San Miguel</t>
-  </si>
-  <si>
-    <t>Cajamarca, provincia: San Pablo</t>
-  </si>
-  <si>
-    <t>Cajamarca, provincia: Santa Cruz</t>
-  </si>
-  <si>
-    <t>Cusco, provincia: Cusco</t>
-  </si>
-  <si>
-    <t>Cusco, provincia: Acomayo</t>
-  </si>
-  <si>
-    <t>Cusco, provincia: Anta</t>
-  </si>
-  <si>
-    <t>Cusco, provincia: Calca</t>
-  </si>
-  <si>
-    <t>Cusco, provincia: Canas</t>
-  </si>
-  <si>
-    <t>Cusco, provincia: Canchis</t>
-  </si>
-  <si>
-    <t>Cusco, provincia: Chumbivilcas</t>
-  </si>
-  <si>
-    <t>Cusco, provincia: Espinar</t>
-  </si>
-  <si>
-    <t>Cusco, provincia: La Convención</t>
-  </si>
-  <si>
-    <t>Cusco, provincia: Paruro</t>
-  </si>
-  <si>
-    <t>Cusco, provincia: Paucartambo</t>
-  </si>
-  <si>
-    <t>Cusco, provincia: Quispicanchi</t>
-  </si>
-  <si>
-    <t>Cusco, provincia: Urubamba</t>
-  </si>
-  <si>
-    <t>Huancavelica, provincia: Huancavelica</t>
-  </si>
-  <si>
-    <t>Huancavelica, provincia: Acobamba</t>
-  </si>
-  <si>
-    <t>Huancavelica, provincia: Angaraes</t>
-  </si>
-  <si>
-    <t>Huancavelica, provincia: Castrovirreyna</t>
-  </si>
-  <si>
-    <t>Huancavelica, provincia: Churcampa</t>
-  </si>
-  <si>
-    <t>Huancavelica, provincia: Huaytará</t>
-  </si>
-  <si>
-    <t>Huancavelica, provincia: Tayacaja</t>
-  </si>
-  <si>
-    <t>Huánuco, provincia: Huánuco</t>
-  </si>
-  <si>
-    <t>Huánuco, provincia: Ambo</t>
-  </si>
-  <si>
-    <t>Huánuco, provincia: Dos De Mayo</t>
-  </si>
-  <si>
-    <t>Huánuco, provincia: Huacaybamba</t>
-  </si>
-  <si>
-    <t>Huánuco, provincia: Huamalíes</t>
-  </si>
-  <si>
-    <t>Huánuco, provincia: Leoncio Prado</t>
-  </si>
-  <si>
-    <t>Huánuco, provincia: Marañón</t>
-  </si>
-  <si>
-    <t>Huánuco, provincia: Pachitea</t>
-  </si>
-  <si>
-    <t>Huánuco, provincia: Puerto Inca</t>
-  </si>
-  <si>
-    <t>Huánuco, provincia: Lauricocha</t>
-  </si>
-  <si>
-    <t>Huánuco, provincia: Yarowilca</t>
-  </si>
-  <si>
-    <t>Ica, provincia: Ica</t>
-  </si>
-  <si>
-    <t>Ica, provincia: Chincha</t>
-  </si>
-  <si>
-    <t>Ica, provincia: Nazca</t>
-  </si>
-  <si>
-    <t>Ica, provincia: Palpa</t>
-  </si>
-  <si>
-    <t>Ica, provincia: Pisco</t>
-  </si>
-  <si>
-    <t>Junín, provincia: Huancayo</t>
-  </si>
-  <si>
-    <t>Junín, provincia: Concepción</t>
-  </si>
-  <si>
-    <t>Junín, provincia: Chanchamayo</t>
-  </si>
-  <si>
-    <t>Junín, provincia: Jauja</t>
-  </si>
-  <si>
-    <t>Junín, provincia: Junín</t>
-  </si>
-  <si>
-    <t>Junín, provincia: Satipo</t>
-  </si>
-  <si>
-    <t>Junín, provincia: Tarma</t>
-  </si>
-  <si>
-    <t>Junín, provincia: Yauli</t>
-  </si>
-  <si>
-    <t>Junín, provincia: Chupaca</t>
-  </si>
-  <si>
-    <t>La Lbertad, provincia: Trujillo</t>
-  </si>
-  <si>
-    <t>La Lbertad, provincia: Ascope</t>
-  </si>
-  <si>
-    <t>La Lbertad, provincia: Bolívar</t>
-  </si>
-  <si>
-    <t>La Lbertad, provincia: Chepén</t>
-  </si>
-  <si>
-    <t>La Lbertad, provincia: Julcán</t>
-  </si>
-  <si>
-    <t>La Lbertad, provincia: Otuzco</t>
-  </si>
-  <si>
-    <t>La Lbertad, provincia: Pacasmayo</t>
-  </si>
-  <si>
-    <t>La Lbertad, provincia: Pataz</t>
-  </si>
-  <si>
-    <t>La Lbertad, provincia: Sánchez Carrión</t>
-  </si>
-  <si>
-    <t>La Lbertad, provincia: Santiago de Chuco</t>
-  </si>
-  <si>
-    <t>La Lbertad, provincia: Gran Chimú</t>
-  </si>
-  <si>
-    <t>La Lbertad, provincia: Virú</t>
-  </si>
-  <si>
-    <t>Lambayeque, provincia: Chiclayo</t>
-  </si>
-  <si>
-    <t>Lambayeque, provincia: Ferreñafe</t>
-  </si>
-  <si>
-    <t>Lambayeque, provincia: Lambayeque</t>
-  </si>
-  <si>
-    <t>Lima, provincia: Lima</t>
-  </si>
-  <si>
-    <t>Lima, provincia: Barranca</t>
-  </si>
-  <si>
-    <t>Lima, provincia: Cajatambo</t>
-  </si>
-  <si>
-    <t>Lima, provincia: Canta</t>
-  </si>
-  <si>
-    <t>Lima, provincia: Cañete</t>
-  </si>
-  <si>
-    <t>Lima, provincia: Huaral</t>
-  </si>
-  <si>
-    <t>Lima, provincia: Huarochirí</t>
-  </si>
-  <si>
-    <t>Lima, provincia: Huaura</t>
-  </si>
-  <si>
-    <t>Lima, provincia: Oyón</t>
-  </si>
-  <si>
-    <t>Lima, provincia: Yauyos</t>
-  </si>
-  <si>
-    <t>Loreto, provincia: Maynas</t>
-  </si>
-  <si>
-    <t>Loreto, provincia: Alto Amazonas</t>
-  </si>
-  <si>
-    <t>Loreto, provincia: Loreto</t>
-  </si>
-  <si>
-    <t>Loreto, provincia: Mariscal Ramón Castilla</t>
-  </si>
-  <si>
-    <t>Loreto, provincia: Requena</t>
-  </si>
-  <si>
-    <t>Loreto, provincia: Ucayali</t>
-  </si>
-  <si>
-    <t>Loreto, provincia: Datem del Marañón</t>
-  </si>
-  <si>
-    <t>Loreto, provincia: Putumayo</t>
-  </si>
-  <si>
-    <t>Madre de Dios prov. de Tambopata</t>
-  </si>
-  <si>
-    <t>Madre de Dios prov. de Manu</t>
-  </si>
-  <si>
-    <t>Madre de Dios prov. de Tahuamanu</t>
-  </si>
-  <si>
-    <t>Moquegua, provincia: Mariscal Nieto</t>
-  </si>
-  <si>
-    <t>Moquegua, provincia: General Sánchez Cerro</t>
-  </si>
-  <si>
-    <t>Moquegua, provincia: Ilo</t>
-  </si>
-  <si>
-    <t>Pasco, provincia: Pasco</t>
-  </si>
-  <si>
-    <t>Pasco, provincia: Daniel Alcides Carrión</t>
-  </si>
-  <si>
-    <t>Pasco, provincia: Oxapampa</t>
-  </si>
-  <si>
-    <t>Piura, provincia: Piura</t>
-  </si>
-  <si>
-    <t>Piura, provincia: Ayabaca</t>
-  </si>
-  <si>
-    <t>Piura, provincia: Huancabamba</t>
-  </si>
-  <si>
-    <t>Piura, provincia: Morropón</t>
-  </si>
-  <si>
-    <t>Piura, provincia: Paita</t>
-  </si>
-  <si>
-    <t>Piura, provincia: Sullana</t>
-  </si>
-  <si>
-    <t>Piura, provincia: Talara</t>
-  </si>
-  <si>
-    <t>Piura, provincia: Sechura</t>
-  </si>
-  <si>
-    <t>Puno, provincia: Puno</t>
-  </si>
-  <si>
-    <t>Puno, provincia: Azángaro</t>
-  </si>
-  <si>
-    <t>Puno, provincia: Carabaya</t>
-  </si>
-  <si>
-    <t>Puno, provincia: Chucuito</t>
-  </si>
-  <si>
-    <t>Puno, provincia: El Collao</t>
-  </si>
-  <si>
-    <t>Puno, provincia: Huancané</t>
-  </si>
-  <si>
-    <t>Puno, provincia: Lampa</t>
-  </si>
-  <si>
-    <t>Puno, provincia: Melgar</t>
-  </si>
-  <si>
-    <t>Puno, provincia: Moho</t>
-  </si>
-  <si>
-    <t>Puno, provincia: San Antonio de Putina</t>
-  </si>
-  <si>
-    <t>Puno, provincia: San Román</t>
-  </si>
-  <si>
-    <t>Puno, provincia: Sandia</t>
-  </si>
-  <si>
-    <t>Puno, provincia: Yunguyo</t>
-  </si>
-  <si>
-    <t>San Martín, provincia: Moyobamba</t>
-  </si>
-  <si>
-    <t>San Martín, provincia: Bellavista</t>
-  </si>
-  <si>
-    <t>San Martín, provincia: El Dorado</t>
-  </si>
-  <si>
-    <t>San Martín, provincia: Huallaga</t>
-  </si>
-  <si>
-    <t>San Martín, provincia: Lamas</t>
-  </si>
-  <si>
-    <t>San Martín, provincia: Mariscal Cáceres</t>
-  </si>
-  <si>
-    <t>San Martín, provincia: Picota</t>
-  </si>
-  <si>
-    <t>San Martín, provincia: Rioja</t>
-  </si>
-  <si>
-    <t>San Martín, provincia: San Martín</t>
-  </si>
-  <si>
-    <t>San Martín, provincia: Tocache</t>
-  </si>
-  <si>
-    <t>Tacna, provincia: Tacna</t>
-  </si>
-  <si>
-    <t>Tacna, provincia: Candarave</t>
-  </si>
-  <si>
-    <t>Tacna, provincia: Jorge Basadre</t>
-  </si>
-  <si>
-    <t>Tacna, provincia: Tarata</t>
-  </si>
-  <si>
-    <t>Tumbes, provincia: Tumbes</t>
-  </si>
-  <si>
-    <t>Tumbes, provincia: Contralmirante Villar</t>
-  </si>
-  <si>
-    <t>Tumbes, provincia: Zarumilla</t>
-  </si>
-  <si>
-    <t>Ucayali, provincia: Coronel Portillo</t>
-  </si>
-  <si>
-    <t>Ucayali, provincia: Atalaya</t>
-  </si>
-  <si>
-    <t>Ucayali, provincia: Padre Abad</t>
-  </si>
-  <si>
-    <t>Ucayali, provincia: Purús</t>
-  </si>
-  <si>
     <t>Ubigeo</t>
   </si>
   <si>
@@ -1219,6 +631,582 @@
   </si>
   <si>
     <t>idh_2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chachapoyas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bagua</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bongara</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Condorcanqui</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Luya</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rodríguez de Mendoza</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Utcubamba</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huaraz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aija</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Antonio Raymondi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Asunción</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bolognesi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carhuaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carlos Fermín Fitzcarrald</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Casma</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Corongo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huari</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huarmey</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huaylas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mariscal Luzuriaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ocros</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pallasca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pomabamba</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Recuay</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Santa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sihuas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yungay</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Abancay</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Andahuaylas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Antabamba</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aymaraes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cotabambas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chincheros</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grau</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arequipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Camaná</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Caravelí</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Castilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Caylloma</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Condesuyos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Islay</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> La Unión</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huamanga</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cangallo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huanca Sancos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huanta</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> La Mar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lucanas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Parinacochas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Páucar del Sara Sara</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sucre</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Víctor Fajardo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vilcas Huamán</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cajamarca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cajabamba</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Celendín</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chota</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Contumazá</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cutervo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hualgayoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jaén</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> San Ignacio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> San Marcos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> San Miguel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> San Pablo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Santa Cruz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cusco</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Acomayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Anta</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Calca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Canas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Canchis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chumbivilcas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Espinar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> La Convención</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paruro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paucartambo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quispicanchi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Urubamba</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huancavelica</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Acobamba</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Angaraes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Castrovirreyna</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Churcampa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huaytará</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tayacaja</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huánuco</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ambo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dos De Mayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huacaybamba</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huamalíes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Leoncio Prado</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marañón</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pachitea</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Puerto Inca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lauricocha</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yarowilca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ica</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chincha</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nazca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Palpa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pisco</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huancayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Concepción</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chanchamayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jauja</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Junín</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Satipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tarma</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yauli</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chupaca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Trujillo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ascope</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bolívar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chepén</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Julcán</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Otuzco</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pacasmayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pataz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sánchez Carrión</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Santiago de Chuco</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gran Chimú</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Virú</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chiclayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ferreñafe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lambayeque</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lima</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barranca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cajatambo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Canta</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cañete</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huaral</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huarochirí</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huaura</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Oyón</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yauyos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Maynas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alto Amazonas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Loreto</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mariscal Ramón Castilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Requena</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ucayali</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Datem del Marañón</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Putumayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mariscal Nieto</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> General Sánchez Cerro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ilo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pasco</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Daniel Alcides Carrión</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Oxapampa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Piura</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ayabaca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huancabamba</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Morropón</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paita</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sullana</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talara</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sechura</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Puno</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Azángaro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carabaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chucuito</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El Collao</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huancané</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lampa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Melgar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Moho</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> San Antonio de Putina</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> San Román</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sandia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yunguyo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Moyobamba</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bellavista</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El Dorado</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huallaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lamas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mariscal Cáceres</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Picota</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rioja</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> San Martín</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tocache</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tacna</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Candarave</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jorge Basadre</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tarata</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tumbes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Contralmirante Villar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zarumilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Coronel Portillo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Atalaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Padre Abad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Purús</t>
   </si>
 </sst>
 </file>
@@ -1227,7 +1215,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="173" formatCode="##\ ###\ ###\ ###\ ##0"/>
+    <numFmt numFmtId="165" formatCode="##\ ###\ ###\ ###\ ##0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1300,7 +1288,7 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1525,13 +1513,13 @@
   <dimension ref="A1:H999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.375" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.625" style="1" customWidth="1"/>
     <col min="5" max="20" width="9.375" style="1" customWidth="1"/>
@@ -1540,22 +1528,22 @@
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>393</v>
+        <v>197</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>394</v>
+        <v>198</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>395</v>
+        <v>199</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>396</v>
+        <v>200</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>397</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1563,7 +1551,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C2" s="4">
         <v>92.048192771084331</v>
@@ -1583,7 +1571,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C3" s="4">
         <v>75.769809771452032</v>
@@ -1604,7 +1592,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C4" s="4">
         <v>91.498169081356465</v>
@@ -1624,7 +1612,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C5" s="4">
         <v>84.356310985206164</v>
@@ -1644,7 +1632,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C6" s="4">
         <v>85.440646691854852</v>
@@ -1664,7 +1652,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C7" s="4">
         <v>86.587918660287087</v>
@@ -1684,7 +1672,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C8" s="4">
         <v>56.343825665859562</v>
@@ -1704,7 +1692,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C9" s="4">
         <v>89.637952559300871</v>
@@ -1724,7 +1712,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C10" s="4">
         <v>92.614770459081839</v>
@@ -1744,7 +1732,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C11" s="4">
         <v>82.784302492122606</v>
@@ -1764,7 +1752,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C12" s="4">
         <v>91.339712918660283</v>
@@ -1784,7 +1772,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C13" s="4">
         <v>89.442231075697208</v>
@@ -1804,7 +1792,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C14" s="4">
         <v>90.627461275925441</v>
@@ -1824,7 +1812,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C15" s="4">
         <v>77.799823633156961</v>
@@ -1844,7 +1832,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C16" s="4">
         <v>80.24803113967593</v>
@@ -1864,7 +1852,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C17" s="4">
         <v>92.725030826140568</v>
@@ -1884,7 +1872,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C18" s="4">
         <v>81.498715188554755</v>
@@ -1904,7 +1892,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C19" s="4">
         <v>84.786324786324784</v>
@@ -1924,7 +1912,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C20" s="4">
         <v>93.156544054747641</v>
@@ -1944,7 +1932,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C21" s="4">
         <v>83.333333333333329</v>
@@ -1964,7 +1952,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C22" s="4">
         <v>84.805653710247356</v>
@@ -1984,7 +1972,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C23" s="4">
         <v>87.661857195708478</v>
@@ -2004,7 +1992,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C24" s="4">
         <v>83.226997985224983</v>
@@ -2024,7 +2012,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C25" s="4">
         <v>87.583892617449663</v>
@@ -2044,7 +2032,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C26" s="4">
         <v>90.560215475647652</v>
@@ -2064,7 +2052,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C27" s="4">
         <v>86.902827429314272</v>
@@ -2084,7 +2072,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C28" s="4">
         <v>92.997955010224942</v>
@@ -2104,7 +2092,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C29" s="4">
         <v>91.55937520423501</v>
@@ -2124,7 +2112,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C30" s="4">
         <v>88.319978632478637</v>
@@ -2144,7 +2132,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C31" s="4">
         <v>93.465539661898575</v>
@@ -2164,7 +2152,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C32" s="4">
         <v>89.703078180332341</v>
@@ -2184,7 +2172,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C33" s="4">
         <v>75.145897699965673</v>
@@ -2204,7 +2192,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C34" s="4">
         <v>87.344532385721209</v>
@@ -2224,7 +2212,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C35" s="4">
         <v>91.845018450184497</v>
@@ -2244,7 +2232,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C36" s="4">
         <v>88.491893522639657</v>
@@ -2264,7 +2252,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C37" s="4">
         <v>70.749339635756982</v>
@@ -2284,7 +2272,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C38" s="4">
         <v>54.329789992221933</v>
@@ -2304,7 +2292,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="C39" s="4">
         <v>89.303339837025135</v>
@@ -2324,7 +2312,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C40" s="4">
         <v>90.848349868394408</v>
@@ -2344,7 +2332,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C41" s="4">
         <v>88.376963350785346</v>
@@ -2364,7 +2352,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C42" s="4">
         <v>87.963433214829863</v>
@@ -2384,7 +2372,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C43" s="4">
         <v>94.804785894206546</v>
@@ -2404,7 +2392,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C44" s="4">
         <v>86.518136335209505</v>
@@ -2424,7 +2412,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C45" s="4">
         <v>92.085441259134342</v>
@@ -2444,7 +2432,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C46" s="4">
         <v>83.682338996444088</v>
@@ -2464,7 +2452,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C47" s="4">
         <v>87.29958985831469</v>
@@ -2484,7 +2472,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C48" s="4">
         <v>84.809417040358738</v>
@@ -2504,7 +2492,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C49" s="4">
         <v>90.587454853689096</v>
@@ -2524,7 +2512,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="C50" s="4">
         <v>77.266535492659301</v>
@@ -2544,7 +2532,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C51" s="4">
         <v>93.307638402242461</v>
@@ -2564,7 +2552,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C52" s="4">
         <v>87.434002111932415</v>
@@ -2584,7 +2572,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C53" s="4">
         <v>85.963545723632961</v>
@@ -2604,7 +2592,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C54" s="4">
         <v>80.634071810542395</v>
@@ -2624,7 +2612,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C55" s="4">
         <v>87.455040591922725</v>
@@ -2644,7 +2632,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C56" s="4">
         <v>85.913978494623649</v>
@@ -2664,7 +2652,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C57" s="4">
         <v>86.430382732794712</v>
@@ -2684,7 +2672,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C58" s="4">
         <v>73.330055719436245</v>
@@ -2704,7 +2692,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C59" s="4">
         <v>76.224961479198768</v>
@@ -2724,7 +2712,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C60" s="4">
         <v>80.712305229038932</v>
@@ -2744,7 +2732,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C61" s="4">
         <v>78.302457259084164</v>
@@ -2764,7 +2752,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C62" s="4">
         <v>88.431069828655311</v>
@@ -2784,7 +2772,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C63" s="4">
         <v>84.180851063829792</v>
@@ -2804,7 +2792,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C64" s="4">
         <v>84.644194756554313</v>
@@ -2824,7 +2812,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C65" s="4">
         <v>91.55457955897154</v>
@@ -2844,7 +2832,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C66" s="4">
         <v>85.976080246913583</v>
@@ -2864,7 +2852,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C67" s="4">
         <v>80.603193376700176</v>
@@ -2883,9 +2871,7 @@
       <c r="A68" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="3" t="s">
-        <v>68</v>
-      </c>
+      <c r="B68" s="3"/>
       <c r="C68" s="4">
         <v>93.631737030126217</v>
       </c>
@@ -2901,10 +2887,10 @@
     </row>
     <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="C69" s="4">
         <v>86.40181991865515</v>
@@ -2921,10 +2907,10 @@
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="C70" s="4">
         <v>92.217642209398193</v>
@@ -2941,10 +2927,10 @@
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="C71" s="4">
         <v>80.873516048658942</v>
@@ -2961,10 +2947,10 @@
     </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C72" s="4">
         <v>89.993188010899189</v>
@@ -2981,10 +2967,10 @@
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="C73" s="4">
         <v>91.927042030134814</v>
@@ -3001,10 +2987,10 @@
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="C74" s="4">
         <v>93.168428529645254</v>
@@ -3021,10 +3007,10 @@
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C75" s="4">
         <v>75.412596833950829</v>
@@ -3041,10 +3027,10 @@
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C76" s="4">
         <v>85.830860534124625</v>
@@ -3061,10 +3047,10 @@
     </row>
     <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C77" s="4">
         <v>92.461767492218158</v>
@@ -3081,10 +3067,10 @@
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C78" s="4">
         <v>85.720338983050851</v>
@@ -3101,10 +3087,10 @@
     </row>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C79" s="4">
         <v>88.120318352059925</v>
@@ -3121,10 +3107,10 @@
     </row>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C80" s="4">
         <v>87.72</v>
@@ -3141,10 +3127,10 @@
     </row>
     <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="C81" s="4">
         <v>82.143358114742597</v>
@@ -3161,10 +3147,10 @@
     </row>
     <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C82" s="4">
         <v>90.273087652327121</v>
@@ -3181,10 +3167,10 @@
     </row>
     <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="C83" s="4">
         <v>79.245283018867923</v>
@@ -3201,10 +3187,10 @@
     </row>
     <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="C84" s="4">
         <v>86.063613006113229</v>
@@ -3221,10 +3207,10 @@
     </row>
     <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C85" s="4">
         <v>92.341085271317823</v>
@@ -3241,10 +3227,10 @@
     </row>
     <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C86" s="4">
         <v>86.809735671290241</v>
@@ -3261,10 +3247,10 @@
     </row>
     <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C87" s="4">
         <v>84.732627228106438</v>
@@ -3281,10 +3267,10 @@
     </row>
     <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C88" s="4">
         <v>85.967226421794933</v>
@@ -3301,10 +3287,10 @@
     </row>
     <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="C89" s="4">
         <v>84.487795857988161</v>
@@ -3321,10 +3307,10 @@
     </row>
     <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C90" s="4">
         <v>77.846377337933532</v>
@@ -3341,10 +3327,10 @@
     </row>
     <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C91" s="4">
         <v>87.2834067547724</v>
@@ -3361,10 +3347,10 @@
     </row>
     <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C92" s="4">
         <v>82.851115129596138</v>
@@ -3381,10 +3367,10 @@
     </row>
     <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C93" s="4">
         <v>86.164888091415619</v>
@@ -3401,10 +3387,10 @@
     </row>
     <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C94" s="4">
         <v>85.020262923791634</v>
@@ -3421,10 +3407,10 @@
     </row>
     <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="C95" s="4">
         <v>85.222222222222229</v>
@@ -3441,10 +3427,10 @@
     </row>
     <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C96" s="4">
         <v>85.215366705471482</v>
@@ -3461,10 +3447,10 @@
     </row>
     <row r="97" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="C97" s="4">
         <v>85.368043087971273</v>
@@ -3481,10 +3467,10 @@
     </row>
     <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="C98" s="4">
         <v>81.474358974358978</v>
@@ -3501,10 +3487,10 @@
     </row>
     <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="C99" s="4">
         <v>86.72394678492239</v>
@@ -3521,10 +3507,10 @@
     </row>
     <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C100" s="4">
         <v>71.426379527645352</v>
@@ -3541,10 +3527,10 @@
     </row>
     <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="C101" s="4">
         <v>56.344938973279085</v>
@@ -3561,10 +3547,10 @@
     </row>
     <row r="102" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C102" s="4">
         <v>86.54732636754764</v>
@@ -3581,10 +3567,10 @@
     </row>
     <row r="103" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C103" s="4">
         <v>57.917928945194163</v>
@@ -3601,10 +3587,10 @@
     </row>
     <row r="104" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="C104" s="4">
         <v>70.06600480034912</v>
@@ -3621,10 +3607,10 @@
     </row>
     <row r="105" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="C105" s="4">
         <v>83.169999610182046</v>
@@ -3641,10 +3627,10 @@
     </row>
     <row r="106" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="C106" s="4">
         <v>88.992828188338009</v>
@@ -3661,10 +3647,10 @@
     </row>
     <row r="107" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="C107" s="4">
         <v>91.255269484026059</v>
@@ -3681,10 +3667,10 @@
     </row>
     <row r="108" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C108" s="4">
         <v>86.139472163359656</v>
@@ -3701,10 +3687,10 @@
     </row>
     <row r="109" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="C109" s="4">
         <v>93.87107548430194</v>
@@ -3721,10 +3707,10 @@
     </row>
     <row r="110" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="C110" s="4">
         <v>88.036669846932426</v>
@@ -3741,10 +3727,10 @@
     </row>
     <row r="111" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="C111" s="4">
         <v>88.091162517728762</v>
@@ -3761,10 +3747,10 @@
     </row>
     <row r="112" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C112" s="4">
         <v>88.421389007243292</v>
@@ -3781,10 +3767,10 @@
     </row>
     <row r="113" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="C113" s="4">
         <v>82.808219178082197</v>
@@ -3801,10 +3787,10 @@
     </row>
     <row r="114" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="C114" s="4">
         <v>84.536979609890722</v>
@@ -3821,10 +3807,10 @@
     </row>
     <row r="115" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="C115" s="4">
         <v>77.92781095819268</v>
@@ -3841,10 +3827,10 @@
     </row>
     <row r="116" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C116" s="4">
         <v>88.423645320197039</v>
@@ -3861,10 +3847,10 @@
     </row>
     <row r="117" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="C117" s="4">
         <v>91.832815588816715</v>
@@ -3881,10 +3867,10 @@
     </row>
     <row r="118" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C118" s="4">
         <v>63.092177745134045</v>
@@ -3901,10 +3887,10 @@
     </row>
     <row r="119" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="C119" s="4">
         <v>87.393111638954863</v>
@@ -3921,10 +3907,10 @@
     </row>
     <row r="120" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="C120" s="4">
         <v>73.695231958762889</v>
@@ -3941,10 +3927,10 @@
     </row>
     <row r="121" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="C121" s="4">
         <v>79.323308270676691</v>
@@ -3961,10 +3947,10 @@
     </row>
     <row r="122" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="C122" s="4">
         <v>66.569266501835614</v>
@@ -3981,10 +3967,10 @@
     </row>
     <row r="123" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="C123" s="4">
         <v>69.144390340852624</v>
@@ -4001,10 +3987,10 @@
     </row>
     <row r="124" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="C124" s="4">
         <v>62.182741116751266</v>
@@ -4021,10 +4007,10 @@
     </row>
     <row r="125" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="C125" s="4">
         <v>63.958632894591304</v>
@@ -4041,10 +4027,10 @@
     </row>
     <row r="126" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C126" s="4">
         <v>93.8153422656667</v>
@@ -4061,10 +4047,10 @@
     </row>
     <row r="127" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C127" s="4">
         <v>90.996484289167213</v>
@@ -4081,10 +4067,10 @@
     </row>
     <row r="128" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="C128" s="4">
         <v>84.755701501154732</v>
@@ -4101,10 +4087,10 @@
     </row>
     <row r="129" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="C129" s="4">
         <v>92.400884096548154</v>
@@ -4121,10 +4107,10 @@
     </row>
     <row r="130" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="C130" s="4">
         <v>85.778297848050684</v>
@@ -4141,10 +4127,10 @@
     </row>
     <row r="131" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="C131" s="4">
         <v>91.912708600770216</v>
@@ -4161,10 +4147,10 @@
     </row>
     <row r="132" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="C132" s="4">
         <v>81.452909032465442</v>
@@ -4181,10 +4167,10 @@
     </row>
     <row r="133" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="C133" s="4">
         <v>80.398445691728853</v>
@@ -4201,10 +4187,10 @@
     </row>
     <row r="134" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="C134" s="4">
         <v>86.508083507527843</v>
@@ -4221,10 +4207,10 @@
     </row>
     <row r="135" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="C135" s="4">
         <v>86.339101444673759</v>
@@ -4241,10 +4227,10 @@
     </row>
     <row r="136" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="C136" s="4">
         <v>88.368609446735661</v>
@@ -4261,10 +4247,10 @@
     </row>
     <row r="137" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="C137" s="4">
         <v>93.069778518694932</v>
@@ -4281,10 +4267,10 @@
     </row>
     <row r="138" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="C138" s="4">
         <v>89.817503110742436</v>
@@ -4301,10 +4287,10 @@
     </row>
     <row r="139" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C139" s="4">
         <v>88.426716543330357</v>
@@ -4321,10 +4307,10 @@
     </row>
     <row r="140" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C140" s="4">
         <v>76.804700615556797</v>
@@ -4341,10 +4327,10 @@
     </row>
     <row r="141" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="C141" s="4">
         <v>82.348089084410233</v>
@@ -4361,10 +4347,10 @@
     </row>
     <row r="142" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="C142" s="4">
         <v>59.809750297265161</v>
@@ -4381,10 +4367,10 @@
     </row>
     <row r="143" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="C143" s="4">
         <v>72.356549981955979</v>
@@ -4401,10 +4387,10 @@
     </row>
     <row r="144" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="C144" s="4">
         <v>63.666407465007779</v>
@@ -4421,10 +4407,10 @@
     </row>
     <row r="145" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="C145" s="4">
         <v>87.323943661971825</v>
@@ -4441,10 +4427,10 @@
     </row>
     <row r="146" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="C146" s="4">
         <v>26.881720430107528</v>
@@ -4461,11 +4447,9 @@
     </row>
     <row r="147" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B147" s="3" t="s">
-        <v>342</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="B147" s="3"/>
       <c r="C147" s="4">
         <v>95.04338046272494</v>
       </c>
@@ -4481,11 +4465,9 @@
     </row>
     <row r="148" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>343</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="B148" s="3"/>
       <c r="C148" s="4">
         <v>60.574749757830155</v>
       </c>
@@ -4501,11 +4483,9 @@
     </row>
     <row r="149" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>344</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="B149" s="3"/>
       <c r="C149" s="4">
         <v>79.958890030832478</v>
       </c>
@@ -4521,10 +4501,10 @@
     </row>
     <row r="150" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C150" s="4">
         <v>93.286121221712293</v>
@@ -4541,10 +4521,10 @@
     </row>
     <row r="151" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C151" s="4">
         <v>83.865750101091791</v>
@@ -4561,10 +4541,10 @@
     </row>
     <row r="152" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C152" s="4">
         <v>86.107958414672908</v>
@@ -4581,10 +4561,10 @@
     </row>
     <row r="153" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C153" s="4">
         <v>53.177467440765732</v>
@@ -4601,10 +4581,10 @@
     </row>
     <row r="154" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C154" s="4">
         <v>77.536009806926145</v>
@@ -4621,10 +4601,10 @@
     </row>
     <row r="155" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C155" s="4">
         <v>89.373405612244895</v>
@@ -4641,10 +4621,10 @@
     </row>
     <row r="156" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C156" s="4">
         <v>78.43733517395863</v>
@@ -4661,10 +4641,10 @@
     </row>
     <row r="157" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C157" s="4">
         <v>86.888418506198974</v>
@@ -4681,10 +4661,10 @@
     </row>
     <row r="158" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C158" s="4">
         <v>87.765930820443515</v>
@@ -4701,10 +4681,10 @@
     </row>
     <row r="159" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C159" s="4">
         <v>81.934996220710502</v>
@@ -4721,10 +4701,10 @@
     </row>
     <row r="160" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C160" s="4">
         <v>73.413575374901342</v>
@@ -4741,10 +4721,10 @@
     </row>
     <row r="161" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C161" s="4">
         <v>59.09033038385639</v>
@@ -4761,10 +4741,10 @@
     </row>
     <row r="162" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C162" s="4">
         <v>26.327257104277912</v>
@@ -4781,10 +4761,10 @@
     </row>
     <row r="163" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C163" s="4">
         <v>26.100113478754256</v>
@@ -4801,10 +4781,10 @@
     </row>
     <row r="164" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C164" s="4">
         <v>83.091467320477989</v>
@@ -4821,10 +4801,10 @@
     </row>
     <row r="165" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C165" s="4">
         <v>88.113924050632917</v>
@@ -4841,10 +4821,10 @@
     </row>
     <row r="166" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C166" s="4">
         <v>79.649001469698277</v>
@@ -4861,10 +4841,10 @@
     </row>
     <row r="167" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C167" s="4">
         <v>83.677786818551667</v>
@@ -4881,10 +4861,10 @@
     </row>
     <row r="168" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C168" s="4">
         <v>88.430547203848462</v>
@@ -4901,10 +4881,10 @@
     </row>
     <row r="169" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C169" s="4">
         <v>82.219677762329269</v>
@@ -4921,10 +4901,10 @@
     </row>
     <row r="170" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C170" s="4">
         <v>89.571899012074638</v>
@@ -4941,10 +4921,10 @@
     </row>
     <row r="171" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C171" s="4">
         <v>89.822105570137069</v>
@@ -4961,10 +4941,10 @@
     </row>
     <row r="172" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C172" s="4">
         <v>87.396528704939925</v>
@@ -4981,10 +4961,10 @@
     </row>
     <row r="173" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C173" s="4">
         <v>81.984013117442103</v>
@@ -5001,10 +4981,10 @@
     </row>
     <row r="174" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C174" s="4">
         <v>88.698967570577906</v>
@@ -5021,10 +5001,10 @@
     </row>
     <row r="175" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C175" s="4">
         <v>77.947103274559197</v>
@@ -5041,10 +5021,10 @@
     </row>
     <row r="176" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C176" s="4">
         <v>80.113149322818444</v>
@@ -5061,10 +5041,10 @@
     </row>
     <row r="177" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C177" s="4">
         <v>91.799919499432832</v>
@@ -5081,10 +5061,10 @@
     </row>
     <row r="178" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C178" s="4">
         <v>58.676418544296332</v>
@@ -5101,10 +5081,10 @@
     </row>
     <row r="179" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C179" s="4">
         <v>81.049883193623742</v>
@@ -5121,10 +5101,10 @@
     </row>
     <row r="180" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C180" s="4">
         <v>97.71042661834953</v>
@@ -5141,10 +5121,10 @@
     </row>
     <row r="181" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C181" s="4">
         <v>87.248152592686168</v>
@@ -5161,10 +5141,10 @@
     </row>
     <row r="182" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C182" s="4">
         <v>91.411346932034022</v>
@@ -5181,10 +5161,10 @@
     </row>
     <row r="183" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C183" s="4">
         <v>66.238532110091739</v>
@@ -5201,10 +5181,10 @@
     </row>
     <row r="184" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C184" s="4">
         <v>87.911139868435242</v>
@@ -5221,10 +5201,10 @@
     </row>
     <row r="185" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C185" s="4">
         <v>90.857813275574202</v>
@@ -5241,10 +5221,10 @@
     </row>
     <row r="186" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C186" s="4">
         <v>81.947977352917036</v>
@@ -5261,10 +5241,10 @@
     </row>
     <row r="187" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C187" s="4">
         <v>92.471642222382769</v>
@@ -5281,10 +5261,10 @@
     </row>
     <row r="188" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C188" s="4">
         <v>90.260869565217391</v>
@@ -5301,10 +5281,10 @@
     </row>
     <row r="189" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C189" s="4">
         <v>80.558659217877093</v>
@@ -5321,10 +5301,10 @@
     </row>
     <row r="190" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C190" s="4">
         <v>86.012658227848107</v>
@@ -5341,10 +5321,10 @@
     </row>
     <row r="191" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C191" s="4">
         <v>68.892686069637804</v>
@@ -5361,10 +5341,10 @@
     </row>
     <row r="192" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C192" s="4">
         <v>12.801608579088471</v>
@@ -5381,10 +5361,10 @@
     </row>
     <row r="193" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C193" s="4">
         <v>56.605513045081587</v>
@@ -5401,10 +5381,10 @@
     </row>
     <row r="194" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C194" s="4">
         <v>94.062887526118203</v>
@@ -5421,10 +5401,10 @@
     </row>
     <row r="195" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C195" s="4">
         <v>84.088356420816169</v>
@@ -5441,10 +5421,10 @@
     </row>
     <row r="196" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C196" s="4">
         <v>79.478729778310367</v>
@@ -5461,10 +5441,10 @@
     </row>
     <row r="197" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C197" s="4">
         <v>100</v>

</xml_diff>